<commit_message>
Adding CSV, Excel and property reader.
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitProject\AllureReportsTestNGSelenium\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD591F2A-87DE-433A-8EE8-EA2988F97373}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA4A73F-0534-4888-9915-A2CA811DE060}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3504" yWindow="3984" windowWidth="10992" windowHeight="8376" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,10 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>https://ui.cogmento.com/</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
   <si>
     <t>Veercraig@gmail.com</t>
   </si>
@@ -50,12 +47,6 @@
     <t>headless</t>
   </si>
   <si>
-    <t>Key</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
     <t>aut</t>
   </si>
   <si>
@@ -63,6 +54,24 @@
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>Pass or fail</t>
+  </si>
+  <si>
+    <t>https://ui.cogmento.com</t>
+  </si>
+  <si>
+    <t>Veercraig1@gmail.com</t>
+  </si>
+  <si>
+    <t>pD@zZVvh7pVWJbS12</t>
+  </si>
+  <si>
+    <t>pD@zZVvh7pVWJbS23</t>
+  </si>
+  <si>
+    <t>Veercraig11@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -86,21 +95,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -108,31 +111,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -448,73 +434,153 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" t="s">
         <v>7</v>
       </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>1</v>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>2</v>
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>4</v>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="b">
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="b">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6" t="b">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{E277D7DD-6AB4-4EEC-90A5-2B8766A01455}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{2E8651F9-3149-488F-8BA7-24A5C01488B2}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{89A2FE0F-8C4B-4918-A8D7-3A7387C7F689}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{2B652BA1-93D8-4421-BBCF-1C6510BAA788}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{FA0E3BAB-B8E5-4532-B5C7-197F8A4DD700}"/>
+    <hyperlink ref="B3" r:id="rId6" xr:uid="{10454161-231F-4548-8D1E-FE62444B1804}"/>
+    <hyperlink ref="C4" r:id="rId7" xr:uid="{5B2E9ED4-D124-4949-9E5D-560E9A7A53AE}"/>
+    <hyperlink ref="C5" r:id="rId8" xr:uid="{0EC838F0-37C9-4C7D-B43E-7257E649CCAE}"/>
+    <hyperlink ref="B5" r:id="rId9" xr:uid="{ECD13E67-2FB4-4103-A5C2-08AEFAB173D2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>